<commit_message>
Charging demand of public stations using traffic counts
</commit_message>
<xml_diff>
--- a/FLPv2/data/excel/results.xlsx
+++ b/FLPv2/data/excel/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\EV-chargers\FLPv2\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2ACEC9-2536-4D91-B81F-ED362E57B156}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CE2B8B-7997-48EA-B0EF-8524CBCB8C5F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8652B31-92E6-46AC-9114-17560BE4FC70}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Fleet size</t>
   </si>
@@ -68,12 +68,15 @@
   <si>
     <t>Approximation (%)</t>
   </si>
+  <si>
+    <t>#Chargers (1000 candidates)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,8 +169,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,8 +239,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -273,15 +316,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1"/>
@@ -308,11 +371,20 @@
     <xf numFmtId="10" fontId="5" fillId="7" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" xfId="5" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
+    <cellStyle name="Bad" xfId="5" builtinId="27"/>
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="6" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="4" builtinId="10"/>
   </cellStyles>
@@ -6801,6 +6873,1613 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="655054720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:view3D>
+      <c:rotX val="10"/>
+      <c:rotY val="20"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="20"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12465524210043352"/>
+          <c:y val="8.9589433799850918E-2"/>
+          <c:w val="0.74864444398088581"/>
+          <c:h val="0.73272331139601543"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:surface3DChart>
+        <c:wireframe val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$36:$F$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$37:$F$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>11491</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7864</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6109</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6109</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4075-4585-B491-89AB3F48D32B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$36:$F$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$38:$F$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>11625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6277</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4075-4585-B491-89AB3F48D32B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$36:$F$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$39:$F$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>11753</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8207</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6458</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6174</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6174</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4075-4585-B491-89AB3F48D32B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$36:$F$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$40:$F$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>13915</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9656</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7596</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6837</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6837</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4075-4585-B491-89AB3F48D32B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:bandFmts>
+          <c:bandFmt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="11"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="12"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="13"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="14"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+        </c:bandFmts>
+        <c:axId val="599795496"/>
+        <c:axId val="599791888"/>
+        <c:axId val="539312344"/>
+      </c:surface3DChart>
+      <c:catAx>
+        <c:axId val="599795496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+                  <a:t> of charging stations</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="599791888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="599791888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="5000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:t>Total driving</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+                  <a:t> time (sec)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="7.8334953020241013E-3"/>
+              <c:y val="0.18493534763041858"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="599795496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="539312344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:t>Fleet size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="599791888"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13230616974958898"/>
+          <c:y val="0.94852695349427041"/>
+          <c:w val="0.73107266560134987"/>
+          <c:h val="5.1473046505729633E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>700</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$36:$F$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$37:$F$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>11491</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7864</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6109</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6109</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8AA4-4131-8F22-D8B9D466A847}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>1000</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$38:$F$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>11625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6277</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8AA4-4131-8F22-D8B9D466A847}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>2000</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$39:$F$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>11753</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8207</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6458</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6174</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6174</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8AA4-4131-8F22-D8B9D466A847}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>3000</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$40:$F$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>13915</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9656</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7596</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6837</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6837</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8AA4-4131-8F22-D8B9D466A847}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="538147592"/>
+        <c:axId val="538148904"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="538147592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> charging stations</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="538148904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="538148904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="14500"/>
+          <c:min val="5000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Total driving</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> time (sec)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="538147592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12708,6 +14387,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -17555,6 +19274,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -21598,13 +23820,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>15272</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>2849</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>13607</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>118</xdr:row>
       <xdr:rowOff>13607</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -21634,13 +23856,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>27216</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>176893</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1102180</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>117</xdr:row>
       <xdr:rowOff>187651</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -21672,13 +23894,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1102179</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>180473</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1442356</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>117</xdr:row>
       <xdr:rowOff>174043</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -21710,13 +23932,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>13607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>146</xdr:row>
       <xdr:rowOff>24365</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -21748,13 +23970,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>13608</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>13608</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1102179</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>146</xdr:row>
       <xdr:rowOff>24366</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -21786,13 +24008,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1102179</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>13607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1469572</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>146</xdr:row>
       <xdr:rowOff>24365</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -21824,13 +24046,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>147</xdr:row>
       <xdr:rowOff>2004</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1102895</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>169</xdr:row>
       <xdr:rowOff>10025</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -21860,13 +24082,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>147</xdr:row>
       <xdr:rowOff>10026</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>169</xdr:row>
       <xdr:rowOff>18047</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -21898,13 +24120,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1102895</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>147</xdr:row>
       <xdr:rowOff>10026</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1463842</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>169</xdr:row>
       <xdr:rowOff>18047</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -21936,13 +24158,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>35826</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>169</xdr:row>
       <xdr:rowOff>162621</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>909460</xdr:colOff>
-      <xdr:row>170</xdr:row>
+      <xdr:row>194</xdr:row>
       <xdr:rowOff>115131</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -21974,13 +24196,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>92927</xdr:colOff>
-      <xdr:row>174</xdr:row>
+      <xdr:row>198</xdr:row>
       <xdr:rowOff>168293</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1548892</xdr:colOff>
-      <xdr:row>199</xdr:row>
+      <xdr:row>223</xdr:row>
       <xdr:rowOff>18209</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22010,13 +24232,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>573298</xdr:colOff>
-      <xdr:row>174</xdr:row>
+      <xdr:row>198</xdr:row>
       <xdr:rowOff>127245</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>503132</xdr:colOff>
-      <xdr:row>199</xdr:row>
+      <xdr:row>223</xdr:row>
       <xdr:rowOff>12484</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22046,13 +24268,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1254512</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>169</xdr:row>
       <xdr:rowOff>147630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>220701</xdr:colOff>
-      <xdr:row>170</xdr:row>
+      <xdr:row>194</xdr:row>
       <xdr:rowOff>92927</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22082,13 +24304,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>11616</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22120,13 +24342,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>46463</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1126738</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>174236</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22158,13 +24380,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1231279</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1544907</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22196,13 +24418,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1774031</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>297656</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>178594</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22225,6 +24447,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>166688</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>15477</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1714500</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>178594</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="22" name="Chart 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{596DB15E-A6CD-4D77-B3CC-964D5EBDBAD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>184546</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1385094</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="23" name="Chart 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3E3D4D5-E851-41D2-AE78-1F2ADF3AF214}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -22530,16 +24824,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE199B32-BAB8-4249-BB01-855BFF420606}">
-  <dimension ref="A1:O68"/>
+  <dimension ref="A1:O92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M63" sqref="M63"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
@@ -23807,52 +26102,145 @@
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
+      <c r="B36" s="29">
+        <v>50</v>
+      </c>
+      <c r="C36" s="29">
+        <v>75</v>
+      </c>
+      <c r="D36" s="29">
+        <v>100</v>
+      </c>
+      <c r="E36" s="29">
+        <v>150</v>
+      </c>
+      <c r="F36" s="29">
+        <v>200</v>
+      </c>
+      <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="30">
+        <v>700</v>
+      </c>
+      <c r="B37" s="1">
+        <v>11491</v>
+      </c>
+      <c r="C37" s="1">
+        <v>7864</v>
+      </c>
+      <c r="D37" s="1">
+        <v>6300</v>
+      </c>
+      <c r="E37" s="24">
+        <v>6109</v>
+      </c>
+      <c r="F37" s="24">
+        <v>6109</v>
+      </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="30">
+        <v>1000</v>
+      </c>
+      <c r="B38" s="1">
+        <v>11625</v>
+      </c>
+      <c r="C38" s="1">
+        <v>8000</v>
+      </c>
+      <c r="D38" s="1">
+        <v>6277</v>
+      </c>
+      <c r="E38" s="24">
+        <v>6006</v>
+      </c>
+      <c r="F38" s="24">
+        <v>6006</v>
+      </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="30">
+        <v>2000</v>
+      </c>
+      <c r="B39" s="1">
+        <v>11753</v>
+      </c>
+      <c r="C39" s="1">
+        <v>8207</v>
+      </c>
+      <c r="D39" s="1">
+        <v>6458</v>
+      </c>
+      <c r="E39" s="24">
+        <v>6174</v>
+      </c>
+      <c r="F39" s="24">
+        <v>6174</v>
+      </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="30">
+        <v>3000</v>
+      </c>
+      <c r="B40" s="1">
+        <v>13915</v>
+      </c>
+      <c r="C40" s="1">
+        <v>9656</v>
+      </c>
+      <c r="D40" s="1">
+        <v>7596</v>
+      </c>
+      <c r="E40" s="24">
+        <v>6837</v>
+      </c>
+      <c r="F40" s="24">
+        <v>6837</v>
+      </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
@@ -23867,6 +26255,12 @@
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
     </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+    </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
     </row>
@@ -23876,11 +26270,23 @@
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
     </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+    </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
@@ -23891,9 +26297,66 @@
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+    </row>
+    <row r="91" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B35:F35"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>